<commit_message>
Added microphone, speaker, and adapter
</commit_message>
<xml_diff>
--- a/BillOfMaterials.xlsx
+++ b/BillOfMaterials.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graemef681\Documents\Uni Project Work 5th Year\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0271F35-BABF-4447-8EFF-9BEE478DF178}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28F506BE-D57C-441F-9DD9-C8216A112877}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Item #</t>
   </si>
@@ -75,9 +69,6 @@
     <t>Dongle</t>
   </si>
   <si>
-    <t>Kirsty</t>
-  </si>
-  <si>
     <t>MY-CAM003M</t>
   </si>
   <si>
@@ -103,12 +94,72 @@
   </si>
   <si>
     <t>Click Here</t>
+  </si>
+  <si>
+    <t>Microphone</t>
+  </si>
+  <si>
+    <t>Tonton High Sensitive Weatherproof Preamp Microphone Audio Pickup Device Sound Voice Pickup Kit for CCTV Security Camera Surveillance</t>
+  </si>
+  <si>
+    <t>Tonton</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>B07KF6SS4Q</t>
+  </si>
+  <si>
+    <t>Security microphone that's small and can listen clearly from quite a distance</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Tonton-Sensitive-Weatherproof-Microphone-Surveillance%EF%BC%8C/dp/B07KF6SS4Q/ref=asc_df_B07KF6SS4Q/?tag=googshopuk-21&amp;linkCode=df0&amp;hvadid=309932293363&amp;hvpos=1o3&amp;hvnetw=g&amp;hvrand=13948887181191337217&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1007336&amp;hvtargid=aud-543776533562:pla-666275186634&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Microphone Adapter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/UGREEN-connecting-Smartphones-Tablets-Turntable-Grey/dp/B00B2HP1MW/ref=asc_df_B00B2HP1MW/?tag=googshopuk-21&amp;linkCode=df0&amp;hvadid=309953091299&amp;hvpos=1o2&amp;hvnetw=g&amp;hvrand=9630926945232197179&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1007336&amp;hvtargid=aud-543776533562:pla-392941865005&amp;psc=1</t>
+  </si>
+  <si>
+    <t>UGREEN RCA 3.5mm Adapter Cable 2 Phono Female to Male Aux Mini Jack Stereo </t>
+  </si>
+  <si>
+    <t>UGREEN</t>
+  </si>
+  <si>
+    <t>B00B2HP1MW</t>
+  </si>
+  <si>
+    <t>Adapter to let microphone input to laptop/computer</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>UKHONK</t>
+  </si>
+  <si>
+    <t>UKHONK Portable USB Speaker with Loud Stereo Sound,USB Powered Stereo Speake</t>
+  </si>
+  <si>
+    <t>B07K85H3V2</t>
+  </si>
+  <si>
+    <t>Speak for system output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.co.uk/UKHONK-Portable-Computer-Notebook-Outdoors/dp/B07K85H3V2/ref=sr_1_8?keywords=usb+speaker&amp;qid=1574845424&amp;s=electronics&amp;sr=1-8 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,13 +282,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,9 +301,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
@@ -558,23 +618,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7EC35D-ED9D-4845-B9BD-9E04E99E038E}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -582,7 +642,7 @@
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +677,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -628,31 +688,31 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -706,43 +766,113 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="8">
+        <v>21.99</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="8">
+        <v>6.99</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="8">
+        <v>10.99</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{F8505BCA-4342-4E3C-805F-CC85F5378934}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K6"/>
+    <hyperlink ref="K8" r:id="rId2"/>
+    <hyperlink ref="K7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the PYNQ board and my components to the list
</commit_message>
<xml_diff>
--- a/BillOfMaterials.xlsx
+++ b/BillOfMaterials.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnade\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124C589D-F7BC-43A1-AAAB-5F1FD17F8EDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Item #</t>
   </si>
@@ -60,15 +66,6 @@
     <t>Camera</t>
   </si>
   <si>
-    <t>Pynq-z2</t>
-  </si>
-  <si>
-    <t>Dans Wifi</t>
-  </si>
-  <si>
-    <t>Dongle</t>
-  </si>
-  <si>
     <t>MY-CAM003M</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>885-MY-CAM003M</t>
   </si>
   <si>
-    <t>£23.75</t>
-  </si>
-  <si>
     <t>Cheap camera that can do up to 120fps</t>
   </si>
   <si>
@@ -114,15 +108,9 @@
     <t>Security microphone that's small and can listen clearly from quite a distance</t>
   </si>
   <si>
-    <t>https://www.amazon.co.uk/Tonton-Sensitive-Weatherproof-Microphone-Surveillance%EF%BC%8C/dp/B07KF6SS4Q/ref=asc_df_B07KF6SS4Q/?tag=googshopuk-21&amp;linkCode=df0&amp;hvadid=309932293363&amp;hvpos=1o3&amp;hvnetw=g&amp;hvrand=13948887181191337217&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1007336&amp;hvtargid=aud-543776533562:pla-666275186634&amp;psc=1</t>
-  </si>
-  <si>
     <t>Microphone Adapter</t>
   </si>
   <si>
-    <t>https://www.amazon.co.uk/UGREEN-connecting-Smartphones-Tablets-Turntable-Grey/dp/B00B2HP1MW/ref=asc_df_B00B2HP1MW/?tag=googshopuk-21&amp;linkCode=df0&amp;hvadid=309953091299&amp;hvpos=1o2&amp;hvnetw=g&amp;hvrand=9630926945232197179&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=1007336&amp;hvtargid=aud-543776533562:pla-392941865005&amp;psc=1</t>
-  </si>
-  <si>
     <t>UGREEN RCA 3.5mm Adapter Cable 2 Phono Female to Male Aux Mini Jack Stereo </t>
   </si>
   <si>
@@ -150,17 +138,116 @@
     <t>Speak for system output</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.amazon.co.uk/UKHONK-Portable-Computer-Notebook-Outdoors/dp/B07K85H3V2/ref=sr_1_8?keywords=usb+speaker&amp;qid=1574845424&amp;s=electronics&amp;sr=1-8 </t>
+    <t>Pmod WiFi</t>
+  </si>
+  <si>
+    <t>Pmod WiFi 802.11g</t>
+  </si>
+  <si>
+    <t>Digilent</t>
+  </si>
+  <si>
+    <t>134-6452</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410-194 </t>
+  </si>
+  <si>
+    <t>WiFi interf for the Logic Fabric of FPGA</t>
+  </si>
+  <si>
+    <t>Wifi USB Dongle</t>
+  </si>
+  <si>
+    <t>Ralink</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>B00JZFT3VS</t>
+  </si>
+  <si>
+    <t>WiFI interf for the PetaLinux OS of PYNQ</t>
+  </si>
+  <si>
+    <t>Amazon Link</t>
+  </si>
+  <si>
+    <t>Pmod PIR Sensor</t>
+  </si>
+  <si>
+    <t>Ralink 5370 USB 2.0 802.11n</t>
+  </si>
+  <si>
+    <t>Passive Infrared Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410-389 </t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>1286-410-389-ND</t>
+  </si>
+  <si>
+    <t>Motion Sensor for FPGA</t>
+  </si>
+  <si>
+    <t>Digi-Key Link</t>
+  </si>
+  <si>
+    <t>RS Store Link</t>
+  </si>
+  <si>
+    <t>Pynq-Z2</t>
+  </si>
+  <si>
+    <t>System-On-Chip dev board</t>
+  </si>
+  <si>
+    <t>TUL/Xilinx</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>1M4-M000127000</t>
+  </si>
+  <si>
+    <t>Farnell Store Link</t>
+  </si>
+  <si>
+    <t>Main hardware dev board</t>
+  </si>
+  <si>
+    <t>Budget Spent</t>
+  </si>
+  <si>
+    <t>Budget Left</t>
+  </si>
+  <si>
+    <t>Used Project Budget?</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +291,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -289,7 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,10 +406,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -318,6 +434,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -618,34 +739,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.5546875" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,10 +801,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -688,191 +815,326 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="13">
+        <v>23.75</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>22</v>
+      <c r="L2" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2913031</v>
+      </c>
+      <c r="I3" s="13">
+        <v>100</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="13">
+        <v>18.45</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="13">
+        <v>6.99</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>24</v>
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="8">
-        <v>21.99</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="13">
+        <v>11.65</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="8">
-        <v>6.99</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="13">
+        <v>21.99</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>31</v>
+        <v>47</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="8">
+        <v>22</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="13">
+        <v>6.99</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="13">
         <v>10.99</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>41</v>
+      <c r="J9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M11" s="14">
+        <f>SUM(I2:I17)-I5-I2-I3</f>
+        <v>70.070000000000022</v>
+      </c>
+      <c r="N11" s="14">
+        <f>500-M11</f>
+        <v>429.92999999999995</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K6"/>
-    <hyperlink ref="K8" r:id="rId2"/>
-    <hyperlink ref="K7"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{99E7B96B-3796-4314-AD9A-88D8E1F35385}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{68808AC4-1F9E-4FE3-B719-D8A56AA74C34}"/>
+    <hyperlink ref="K4" r:id="rId6" xr:uid="{9D2C0792-9022-430B-B1E8-9A25B9703C3F}"/>
+    <hyperlink ref="K3" r:id="rId7" xr:uid="{37F73EBD-6D39-417C-BA0A-C2977A33EAC9}"/>
+    <hyperlink ref="K8" r:id="rId8" xr:uid="{75890A76-29C2-4AF9-888A-19F60F7C35E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to include camera connector
</commit_message>
<xml_diff>
--- a/BillOfMaterials.xlsx
+++ b/BillOfMaterials.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>Item #</t>
   </si>
@@ -232,6 +232,38 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Camera Connector</t>
+  </si>
+  <si>
+    <t>1 pc FPC FFC Cable Connector 24 PIN 0.5 mm Adapter to 24 Position 2.54 mm 1.00 inch pitch through hole DIP PCB</t>
+  </si>
+  <si>
+    <t>RTLECS</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF151515"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>FPC24P05T254</t>
+    </r>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>Connector for Camera to FPGA</t>
+  </si>
+  <si>
+    <t>AliExpress Link</t>
   </si>
 </sst>
 </file>
@@ -241,7 +273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +320,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF151515"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +352,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +423,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,6 +449,9 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -720,7 +767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -731,7 +778,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +786,7 @@
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
@@ -747,12 +794,12 @@
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="75.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +833,7 @@
       <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1018,7 +1065,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1094,7 +1141,44 @@
         <v>68</v>
       </c>
     </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10">
+        <v>3.58</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="13"/>
       <c r="F11" s="12" t="s">
         <v>64</v>
       </c>
@@ -1105,11 +1189,11 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F12" s="11">
         <f>SUM(I2:I17)-I5-I2-I3</f>
-        <v>70.070000000000022</v>
+        <v>73.650000000000034</v>
       </c>
       <c r="G12" s="11">
         <f>500-F12</f>
-        <v>429.92999999999995</v>
+        <v>426.34999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -1122,8 +1206,9 @@
     <hyperlink ref="K4" r:id="rId6"/>
     <hyperlink ref="K3" r:id="rId7"/>
     <hyperlink ref="K8" r:id="rId8"/>
+    <hyperlink ref="K10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for final report
</commit_message>
<xml_diff>
--- a/BillOfMaterials.xlsx
+++ b/BillOfMaterials.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>Item #</t>
   </si>
@@ -99,9 +99,6 @@
     <t>B07KF6SS4Q</t>
   </si>
   <si>
-    <t>Security microphone that's small and can listen clearly from quite a distance</t>
-  </si>
-  <si>
     <t>Microphone Adapter</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>B00B2HP1MW</t>
   </si>
   <si>
-    <t>Adapter to let microphone input to laptop/computer</t>
-  </si>
-  <si>
     <t>Speaker</t>
   </si>
   <si>
@@ -198,22 +192,7 @@
     <t>RS Store Link</t>
   </si>
   <si>
-    <t>Pynq-Z2</t>
-  </si>
-  <si>
     <t>System-On-Chip dev board</t>
-  </si>
-  <si>
-    <t>TUL/Xilinx</t>
-  </si>
-  <si>
-    <t>Farnell</t>
-  </si>
-  <si>
-    <t>1M4-M000127000</t>
-  </si>
-  <si>
-    <t>Farnell Store Link</t>
   </si>
   <si>
     <t>Main hardware dev board</t>
@@ -265,15 +244,88 @@
   <si>
     <t>AliExpress Link</t>
   </si>
+  <si>
+    <t>Other Expenditure:</t>
+  </si>
+  <si>
+    <t>Zybo-Z7-20</t>
+  </si>
+  <si>
+    <t>Digilent Store Link</t>
+  </si>
+  <si>
+    <t>Xilinx/Digilent</t>
+  </si>
+  <si>
+    <t>410-351-20</t>
+  </si>
+  <si>
+    <t>TONOR</t>
+  </si>
+  <si>
+    <t>B07H3KLHNJ</t>
+  </si>
+  <si>
+    <t>TONOR Conference USB Microphone, Omnidirectional Condenser PC Mic for Video Conference, Recording, Skype, Online Class, Court Reporter, Plug &amp; Play Compatible with Mac OS X Windows PC Compute</t>
+  </si>
+  <si>
+    <t>Camera Tripod</t>
+  </si>
+  <si>
+    <t>Microphone that did not work</t>
+  </si>
+  <si>
+    <t>Connector for above microphone</t>
+  </si>
+  <si>
+    <t>Total Product Cost</t>
+  </si>
+  <si>
+    <t>Final Product:</t>
+  </si>
+  <si>
+    <t>Conference microphone for user interaction system. It is no longer available on Amazon so the price is an estimate based on records from logbook</t>
+  </si>
+  <si>
+    <t>External Power Supply</t>
+  </si>
+  <si>
+    <t>BENSN AC Power Adapter, Universal 5V 3A (Compatible with 2.5A / 2A / 1A etc.) DC Power Supply with 4 Selectable Adapter Tips</t>
+  </si>
+  <si>
+    <t>BENSN</t>
+  </si>
+  <si>
+    <t>B07JZ25BKH</t>
+  </si>
+  <si>
+    <t>External power supply required for combined FPGA design</t>
+  </si>
+  <si>
+    <t>K&amp;F Concept Heavy Duty Light Stand, Adjustable Height 79’’/2m 891g Aluminum Magnesium Alloy for Photographic Equipment Softbox Umbrellas with Case</t>
+  </si>
+  <si>
+    <t>K&amp;F</t>
+  </si>
+  <si>
+    <t>B07R4TF3L4</t>
+  </si>
+  <si>
+    <t>2m tripod for camera (used in creating dataset)</t>
+  </si>
+  <si>
+    <t>SRL09</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,8 +378,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,8 +429,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -415,21 +489,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -452,9 +587,56 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,424 +973,615 @@
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
     <col min="10" max="10" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
     <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="75.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" s="13" customFormat="1" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="57" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L2" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="9">
+        <v>23.75</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="9">
+        <v>241.3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="9">
+        <v>18.45</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="9">
+        <v>6.99</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="9">
+        <v>11.65</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="32">
+        <v>20</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="9">
+        <v>10.99</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="H10" s="8"/>
+      <c r="I10" s="9">
+        <v>3.58</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="E11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="9">
+        <v>13.99</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="12"/>
+      <c r="F12" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F13" s="10">
+        <f>SUM(I3:I11)</f>
+        <v>350.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:13" s="21" customFormat="1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" ht="57" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="10">
-        <v>23.75</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D16" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="9">
+        <v>21.99</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="9">
+        <v>6.99</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="29">
+        <v>34.99</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="G20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2913031</v>
-      </c>
-      <c r="I3" s="10">
-        <v>100</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="10">
-        <v>18.45</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="10">
-        <v>6.99</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="10">
-        <v>11.65</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="86.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="10">
-        <v>21.99</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="10">
-        <v>6.99</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="10">
-        <v>10.99</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10">
-        <v>3.58</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
-      <c r="F11" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F12" s="11">
-        <f>SUM(I2:I17)-I5-I2-I3</f>
-        <v>73.650000000000034</v>
-      </c>
-      <c r="G12" s="11">
-        <f>500-F12</f>
-        <v>426.34999999999997</v>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="10">
+        <f>SUM(I4,I5,I7,I8,I9,I17,I18,I19)</f>
+        <v>366.36</v>
+      </c>
+      <c r="G21" s="10">
+        <f>500-F21</f>
+        <v>133.63999999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId1"/>
     <hyperlink ref="K9" r:id="rId2"/>
-    <hyperlink ref="K7" r:id="rId3"/>
-    <hyperlink ref="K5" r:id="rId4"/>
-    <hyperlink ref="K6" r:id="rId5"/>
-    <hyperlink ref="K4" r:id="rId6"/>
-    <hyperlink ref="K3" r:id="rId7"/>
-    <hyperlink ref="K8" r:id="rId8"/>
+    <hyperlink ref="K17" r:id="rId3"/>
+    <hyperlink ref="K6" r:id="rId4"/>
+    <hyperlink ref="K7" r:id="rId5"/>
+    <hyperlink ref="K5" r:id="rId6"/>
+    <hyperlink ref="K4" r:id="rId7" display="Xilinx Store Link"/>
+    <hyperlink ref="K18" r:id="rId8"/>
     <hyperlink ref="K10" r:id="rId9"/>
+    <hyperlink ref="K8" r:id="rId10"/>
+    <hyperlink ref="K11" r:id="rId11"/>
+    <hyperlink ref="K19" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>